<commit_message>
Added Data Results for 4000 elements
</commit_message>
<xml_diff>
--- a/HybridAlgorithmResults.xlsx
+++ b/HybridAlgorithmResults.xlsx
@@ -406,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -438,6 +438,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -445,60 +502,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,7 +787,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,97 +800,103 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
-      <c r="C3" s="18">
+      <c r="C3" s="15">
         <v>2000</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="16">
         <v>4000</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="16">
         <v>6000</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <v>8000</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="16">
         <v>10000</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="16">
         <v>12000</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="16">
         <v>14000</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="16">
         <v>16000</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="17">
         <v>18000</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="18">
         <v>6.4048199999999991</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
+      <c r="D4" s="19">
+        <v>24.922080000000001</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="21">
         <v>2.0217599999999996</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="28"/>
+      <c r="D5" s="11">
+        <v>3.7152400000000001</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="2:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="23">
         <v>1.1597200000000001</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
+      <c r="D6" s="24">
+        <v>2.0771000000000002</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4">
@@ -896,73 +905,79 @@
       <c r="D9" s="5">
         <v>1.1128</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="30" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="H9" s="5">
-        <v>3.5375999999999999</v>
+        <v>1.9626999999999999</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="6">
         <v>2</v>
       </c>
       <c r="D10" s="7">
         <v>1.1745000000000001</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="6">
         <v>2</v>
       </c>
       <c r="H10" s="7">
-        <v>3.6453000000000002</v>
+        <v>2.625</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="6">
         <v>3</v>
       </c>
       <c r="D11" s="7">
         <v>1.0495000000000001</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="6">
         <v>3</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <v>2.04</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="6">
         <v>4</v>
       </c>
       <c r="D12" s="7">
         <v>1.18</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="6">
         <v>4</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <v>1.8332999999999999</v>
+      </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
       <c r="D13" s="9">
         <v>1.2818000000000001</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="8">
         <v>5</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9">
+        <v>1.9245000000000001</v>
+      </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="10">
@@ -971,12 +986,12 @@
       </c>
       <c r="H14" s="10">
         <f>AVERAGE(H9:H13)</f>
-        <v>3.59145</v>
+        <v>2.0771000000000002</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="4">
@@ -985,7 +1000,7 @@
       <c r="D16" s="5">
         <v>6.3722000000000003</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="30" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="4">
@@ -996,14 +1011,14 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="6">
         <v>2</v>
       </c>
       <c r="D17" s="7">
         <v>6.2575000000000003</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="6">
         <v>2</v>
       </c>
@@ -1012,46 +1027,52 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="6">
         <v>3</v>
       </c>
       <c r="D18" s="7">
         <v>6.3083</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="6">
         <v>3</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7">
+        <v>24.928100000000001</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="6">
         <v>4</v>
       </c>
       <c r="D19" s="7">
         <v>6.9898999999999996</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="6">
         <v>4</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7">
+        <v>26.6373</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="8">
         <v>5</v>
       </c>
       <c r="D20" s="9">
         <v>6.0961999999999996</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="8">
         <v>5</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="9">
+        <v>25.072199999999999</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="10">
@@ -1060,12 +1081,12 @@
       </c>
       <c r="H21" s="10">
         <f>AVERAGE(H16:H20)</f>
-        <v>23.9864</v>
+        <v>24.922080000000001</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="4">
@@ -1074,73 +1095,79 @@
       <c r="D23" s="5">
         <v>2.1343999999999999</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="30" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>1.9626999999999999</v>
+        <v>3.5375999999999999</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="6">
         <v>2</v>
       </c>
       <c r="D24" s="7">
         <v>2.0802999999999998</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="6">
         <v>2</v>
       </c>
       <c r="H24" s="7">
-        <v>2.625</v>
+        <v>3.6453000000000002</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="6">
         <v>3</v>
       </c>
       <c r="D25" s="7">
         <v>1.9058999999999999</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="6">
         <v>3</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="26">
+        <v>3.72</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="6">
         <v>4</v>
       </c>
       <c r="D26" s="7">
         <v>2.0171000000000001</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="6">
         <v>4</v>
       </c>
-      <c r="H26" s="7"/>
+      <c r="H26" s="26">
+        <v>3.7803</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="8">
         <v>5</v>
       </c>
       <c r="D27" s="9">
         <v>1.9711000000000001</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="8">
         <v>5</v>
       </c>
-      <c r="H27" s="9"/>
+      <c r="H27" s="9">
+        <v>3.8929999999999998</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="10">
@@ -1149,7 +1176,7 @@
       </c>
       <c r="H28" s="10">
         <f>AVERAGE(H23:H27)</f>
-        <v>2.2938499999999999</v>
+        <v>3.7152400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformatted the names of Data Screenshots and Added Hybrid Sorting Algorithm Test Results for 6000 elements
</commit_message>
<xml_diff>
--- a/HybridAlgorithmResults.xlsx
+++ b/HybridAlgorithmResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Bubble</t>
   </si>
@@ -51,6 +51,36 @@
   </si>
   <si>
     <t>Merge (4000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Hybrid (6000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Bubble (6000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Merge (6000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Hybrid (8000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Bubble (8000 elements) in ms</t>
+  </si>
+  <si>
+    <t>Merge (8000 elements) in ms</t>
+  </si>
+  <si>
+    <t>2000 Elements</t>
+  </si>
+  <si>
+    <t>4000 Elements</t>
+  </si>
+  <si>
+    <t>6000 Elements</t>
+  </si>
+  <si>
+    <t>8000 Elements</t>
   </si>
 </sst>
 </file>
@@ -406,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -502,6 +532,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,21 +841,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K28"/>
+  <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="11" width="13.85546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="20.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="27"/>
       <c r="D2" s="28"/>
@@ -810,7 +866,7 @@
       <c r="J2" s="28"/>
       <c r="K2" s="29"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="15">
         <v>2000</v>
@@ -840,7 +896,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
@@ -858,7 +914,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
@@ -876,7 +932,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="2:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
@@ -886,7 +942,9 @@
       <c r="D6" s="24">
         <v>2.0771000000000002</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="24">
+        <v>3.1892399999999999</v>
+      </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -894,300 +952,594 @@
       <c r="J6" s="24"/>
       <c r="K6" s="25"/>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="F8" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
+      <c r="N8" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="35"/>
+      <c r="P8" s="36"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="41"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="41"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <v>1.1128</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F10" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H10" s="5">
         <v>1.9626999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="6">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7">
-        <v>1.1745000000000001</v>
-      </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="6">
-        <v>2</v>
-      </c>
-      <c r="H10" s="7">
-        <v>2.625</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>3.2054999999999998</v>
+      </c>
+      <c r="N10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="31"/>
       <c r="C11" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="7">
-        <v>1.0495000000000001</v>
+        <v>1.1745000000000001</v>
       </c>
       <c r="F11" s="31"/>
       <c r="G11" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" s="7">
-        <v>2.04</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+        <v>2.625</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="6">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7">
+        <v>3.1863000000000001</v>
+      </c>
+      <c r="N11" s="31"/>
+      <c r="O11" s="6">
+        <v>2</v>
+      </c>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="31"/>
       <c r="C12" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="7">
-        <v>1.18</v>
+        <v>1.0495000000000001</v>
       </c>
       <c r="F12" s="31"/>
       <c r="G12" s="6">
+        <v>3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2.04</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="6">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7">
+        <v>3.2174999999999998</v>
+      </c>
+      <c r="N12" s="31"/>
+      <c r="O12" s="6">
+        <v>3</v>
+      </c>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="C13" s="6">
         <v>4</v>
       </c>
-      <c r="H12" s="7">
+      <c r="D13" s="7">
+        <v>1.18</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="6">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7">
         <v>1.8332999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="32"/>
-      <c r="C13" s="8">
+      <c r="J13" s="31"/>
+      <c r="K13" s="6">
+        <v>4</v>
+      </c>
+      <c r="L13" s="7">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="N13" s="31"/>
+      <c r="O13" s="6">
+        <v>4</v>
+      </c>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="32"/>
+      <c r="C14" s="8">
         <v>5</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D14" s="9">
         <v>1.2818000000000001</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="8">
+      <c r="F14" s="32"/>
+      <c r="G14" s="8">
         <v>5</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H14" s="9">
         <v>1.9245000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="10">
-        <f>AVERAGE(D9:D13)</f>
+      <c r="J14" s="32"/>
+      <c r="K14" s="8">
+        <v>5</v>
+      </c>
+      <c r="L14" s="9">
+        <v>3.1328999999999998</v>
+      </c>
+      <c r="N14" s="32"/>
+      <c r="O14" s="8">
+        <v>5</v>
+      </c>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="10">
+        <f>AVERAGE(D10:D14)</f>
         <v>1.1597200000000001</v>
       </c>
-      <c r="H14" s="10">
-        <f>AVERAGE(H9:H13)</f>
+      <c r="F15" s="3"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="10">
+        <f>AVERAGE(H10:H14)</f>
         <v>2.0771000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="30" t="s">
+      <c r="J15" s="3"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="10">
+        <f>AVERAGE(L10:L14)</f>
+        <v>3.1892399999999999</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="10" t="e">
+        <f>AVERAGE(P10:P14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="26"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="26"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="26"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="5">
         <v>6.3722000000000003</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F17" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H17" s="5">
         <v>24.009399999999999</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="C17" s="6">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7">
-        <v>6.2575000000000003</v>
-      </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="6">
-        <v>2</v>
-      </c>
-      <c r="H17" s="7">
-        <v>23.9634</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5">
+        <v>55.846400000000003</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="31"/>
       <c r="C18" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="7">
-        <v>6.3083</v>
+        <v>6.2575000000000003</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="7">
-        <v>24.928100000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>23.9634</v>
+      </c>
+      <c r="J18" s="31"/>
+      <c r="K18" s="6">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="6">
+        <v>2</v>
+      </c>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="31"/>
       <c r="C19" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="7">
-        <v>6.9898999999999996</v>
+        <v>6.3083</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="6">
+        <v>3</v>
+      </c>
+      <c r="H19" s="7">
+        <v>24.928100000000001</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="K19" s="6">
+        <v>3</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="6">
+        <v>3</v>
+      </c>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="31"/>
+      <c r="C20" s="6">
         <v>4</v>
       </c>
-      <c r="H19" s="7">
+      <c r="D20" s="7">
+        <v>6.9898999999999996</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="7">
         <v>26.6373</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="32"/>
-      <c r="C20" s="8">
+      <c r="J20" s="31"/>
+      <c r="K20" s="6">
+        <v>4</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="6">
+        <v>4</v>
+      </c>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="32"/>
+      <c r="C21" s="8">
         <v>5</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D21" s="9">
         <v>6.0961999999999996</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="8">
+      <c r="F21" s="32"/>
+      <c r="G21" s="8">
         <v>5</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H21" s="9">
         <v>25.072199999999999</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="10">
-        <f>AVERAGE(D16:D20)</f>
+      <c r="J21" s="32"/>
+      <c r="K21" s="8">
+        <v>5</v>
+      </c>
+      <c r="L21" s="9"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="8">
+        <v>5</v>
+      </c>
+      <c r="P21" s="9"/>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="10">
+        <f>AVERAGE(D17:D21)</f>
         <v>6.4048199999999991</v>
       </c>
-      <c r="H21" s="10">
-        <f>AVERAGE(H16:H20)</f>
+      <c r="F22" s="3"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="10">
+        <f>AVERAGE(H17:H21)</f>
         <v>24.922080000000001</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+      <c r="J22" s="3"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="10">
+        <f>AVERAGE(L17:L21)</f>
+        <v>55.846400000000003</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="10" t="e">
+        <f>AVERAGE(P17:P21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="26"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="26"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="26"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="26"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C24" s="4">
         <v>1</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D24" s="5">
         <v>2.1343999999999999</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F24" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G24" s="4">
         <v>1</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H24" s="5">
         <v>3.5375999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="C24" s="6">
-        <v>2</v>
-      </c>
-      <c r="D24" s="7">
-        <v>2.0802999999999998</v>
-      </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="6">
-        <v>2</v>
-      </c>
-      <c r="H24" s="7">
-        <v>3.6453000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="N24" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="4">
+        <v>1</v>
+      </c>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="31"/>
       <c r="C25" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="7">
-        <v>1.9058999999999999</v>
+        <v>2.0802999999999998</v>
       </c>
       <c r="F25" s="31"/>
       <c r="G25" s="6">
-        <v>3</v>
-      </c>
-      <c r="H25" s="26">
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H25" s="7">
+        <v>3.6453000000000002</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="6">
+        <v>2</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="6">
+        <v>2</v>
+      </c>
+      <c r="P25" s="7"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="31"/>
       <c r="C26" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="7">
-        <v>2.0171000000000001</v>
+        <v>1.9058999999999999</v>
       </c>
       <c r="F26" s="31"/>
       <c r="G26" s="6">
+        <v>3</v>
+      </c>
+      <c r="H26" s="26">
+        <v>3.72</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="6">
+        <v>3</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="6">
+        <v>3</v>
+      </c>
+      <c r="P26" s="26"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="31"/>
+      <c r="C27" s="6">
         <v>4</v>
       </c>
-      <c r="H26" s="26">
+      <c r="D27" s="7">
+        <v>2.0171000000000001</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="G27" s="6">
+        <v>4</v>
+      </c>
+      <c r="H27" s="26">
         <v>3.7803</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="32"/>
-      <c r="C27" s="8">
+      <c r="J27" s="31"/>
+      <c r="K27" s="6">
+        <v>4</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="6">
+        <v>4</v>
+      </c>
+      <c r="P27" s="26"/>
+    </row>
+    <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="32"/>
+      <c r="C28" s="8">
         <v>5</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="9">
         <v>1.9711000000000001</v>
       </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="8">
+      <c r="F28" s="32"/>
+      <c r="G28" s="8">
         <v>5</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H28" s="9">
         <v>3.8929999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="10">
-        <f>AVERAGE(D23:D27)</f>
+      <c r="J28" s="32"/>
+      <c r="K28" s="8">
+        <v>5</v>
+      </c>
+      <c r="L28" s="9"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="8">
+        <v>5</v>
+      </c>
+      <c r="P28" s="9"/>
+    </row>
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="10">
+        <f>AVERAGE(D24:D28)</f>
         <v>2.0217599999999996</v>
       </c>
-      <c r="H28" s="10">
-        <f>AVERAGE(H23:H27)</f>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="10">
+        <f>AVERAGE(H24:H28)</f>
         <v>3.7152400000000001</v>
       </c>
+      <c r="J29" s="37"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="10" t="e">
+        <f>AVERAGE(L24:L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N29" s="37"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="10" t="e">
+        <f>AVERAGE(P24:P28)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="17">
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="N10:N14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="N24:N28"/>
     <mergeCell ref="C2:K2"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="J10:J14"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="J8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the 6000 element dataset test results for the Hybrid Sorting Algorithm
</commit_message>
<xml_diff>
--- a/HybridAlgorithmResults.xlsx
+++ b/HybridAlgorithmResults.xlsx
@@ -516,6 +516,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,42 +559,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,15 +856,15 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
@@ -954,43 +954,43 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
-      <c r="F8" s="34" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="F8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
-      <c r="J8" s="34" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+      <c r="J8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
-      <c r="N8" s="34" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
+      <c r="N8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="36"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="41"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="41"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="35"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4">
@@ -999,7 +999,7 @@
       <c r="D10" s="5">
         <v>1.1128</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="4">
@@ -1008,7 +1008,7 @@
       <c r="H10" s="5">
         <v>1.9626999999999999</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="36" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="4">
@@ -1017,7 +1017,7 @@
       <c r="L10" s="5">
         <v>3.2054999999999998</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="N10" s="36" t="s">
         <v>12</v>
       </c>
       <c r="O10" s="4">
@@ -1026,112 +1026,112 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="7">
         <v>1.1745000000000001</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="6">
         <v>2</v>
       </c>
       <c r="H11" s="7">
         <v>2.625</v>
       </c>
-      <c r="J11" s="31"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="6">
         <v>2</v>
       </c>
       <c r="L11" s="7">
         <v>3.1863000000000001</v>
       </c>
-      <c r="N11" s="31"/>
+      <c r="N11" s="37"/>
       <c r="O11" s="6">
         <v>2</v>
       </c>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="6">
         <v>3</v>
       </c>
       <c r="D12" s="7">
         <v>1.0495000000000001</v>
       </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="6">
         <v>3</v>
       </c>
       <c r="H12" s="7">
         <v>2.04</v>
       </c>
-      <c r="J12" s="31"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="6">
         <v>3</v>
       </c>
       <c r="L12" s="7">
         <v>3.2174999999999998</v>
       </c>
-      <c r="N12" s="31"/>
+      <c r="N12" s="37"/>
       <c r="O12" s="6">
         <v>3</v>
       </c>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="6">
         <v>4</v>
       </c>
       <c r="D13" s="7">
         <v>1.18</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="6">
         <v>4</v>
       </c>
       <c r="H13" s="7">
         <v>1.8332999999999999</v>
       </c>
-      <c r="J13" s="31"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="6">
         <v>4</v>
       </c>
       <c r="L13" s="7">
         <v>3.2040000000000002</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="37"/>
       <c r="O13" s="6">
         <v>4</v>
       </c>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="8">
         <v>5</v>
       </c>
       <c r="D14" s="9">
         <v>1.2818000000000001</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="8">
         <v>5</v>
       </c>
       <c r="H14" s="9">
         <v>1.9245000000000001</v>
       </c>
-      <c r="J14" s="32"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="8">
         <v>5</v>
       </c>
       <c r="L14" s="9">
         <v>3.1328999999999998</v>
       </c>
-      <c r="N14" s="32"/>
+      <c r="N14" s="38"/>
       <c r="O14" s="8">
         <v>5</v>
       </c>
@@ -1139,25 +1139,25 @@
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="33"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="10">
         <f>AVERAGE(D10:D14)</f>
         <v>1.1597200000000001</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="33"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="10">
         <f>AVERAGE(H10:H14)</f>
         <v>2.0771000000000002</v>
       </c>
       <c r="J15" s="3"/>
-      <c r="K15" s="33"/>
+      <c r="K15" s="27"/>
       <c r="L15" s="10">
         <f>AVERAGE(L10:L14)</f>
         <v>3.1892399999999999</v>
       </c>
       <c r="N15" s="3"/>
-      <c r="O15" s="33"/>
+      <c r="O15" s="27"/>
       <c r="P15" s="10" t="e">
         <f>AVERAGE(P10:P14)</f>
         <v>#DIV/0!</v>
@@ -1165,20 +1165,20 @@
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="26"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="33"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="26"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="33"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="26"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="33"/>
+      <c r="O16" s="27"/>
       <c r="P16" s="26"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="4">
@@ -1187,7 +1187,7 @@
       <c r="D17" s="5">
         <v>6.3722000000000003</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="36" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="4">
@@ -1196,7 +1196,7 @@
       <c r="H17" s="5">
         <v>24.009399999999999</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="36" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="4">
@@ -1205,7 +1205,7 @@
       <c r="L17" s="5">
         <v>55.846400000000003</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="O17" s="4">
@@ -1214,104 +1214,104 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="7">
         <v>6.2575000000000003</v>
       </c>
-      <c r="F18" s="31"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="6">
         <v>2</v>
       </c>
       <c r="H18" s="7">
         <v>23.9634</v>
       </c>
-      <c r="J18" s="31"/>
+      <c r="J18" s="37"/>
       <c r="K18" s="6">
         <v>2</v>
       </c>
       <c r="L18" s="7"/>
-      <c r="N18" s="31"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="6">
         <v>2</v>
       </c>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="6">
         <v>3</v>
       </c>
       <c r="D19" s="7">
         <v>6.3083</v>
       </c>
-      <c r="F19" s="31"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="6">
         <v>3</v>
       </c>
       <c r="H19" s="7">
         <v>24.928100000000001</v>
       </c>
-      <c r="J19" s="31"/>
+      <c r="J19" s="37"/>
       <c r="K19" s="6">
         <v>3</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="N19" s="31"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="6">
         <v>3</v>
       </c>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="6">
         <v>4</v>
       </c>
       <c r="D20" s="7">
         <v>6.9898999999999996</v>
       </c>
-      <c r="F20" s="31"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="6">
         <v>4</v>
       </c>
       <c r="H20" s="7">
         <v>26.6373</v>
       </c>
-      <c r="J20" s="31"/>
+      <c r="J20" s="37"/>
       <c r="K20" s="6">
         <v>4</v>
       </c>
       <c r="L20" s="7"/>
-      <c r="N20" s="31"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="6">
         <v>4</v>
       </c>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="32"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="8">
         <v>5</v>
       </c>
       <c r="D21" s="9">
         <v>6.0961999999999996</v>
       </c>
-      <c r="F21" s="32"/>
+      <c r="F21" s="38"/>
       <c r="G21" s="8">
         <v>5</v>
       </c>
       <c r="H21" s="9">
         <v>25.072199999999999</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="8">
         <v>5</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="N21" s="32"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="8">
         <v>5</v>
       </c>
@@ -1319,25 +1319,25 @@
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="10">
         <f>AVERAGE(D17:D21)</f>
         <v>6.4048199999999991</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="33"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="10">
         <f>AVERAGE(H17:H21)</f>
         <v>24.922080000000001</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="33"/>
+      <c r="K22" s="27"/>
       <c r="L22" s="10">
         <f>AVERAGE(L17:L21)</f>
         <v>55.846400000000003</v>
       </c>
       <c r="N22" s="3"/>
-      <c r="O22" s="33"/>
+      <c r="O22" s="27"/>
       <c r="P22" s="10" t="e">
         <f>AVERAGE(P17:P21)</f>
         <v>#DIV/0!</v>
@@ -1345,20 +1345,20 @@
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="26"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="33"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="26"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="33"/>
+      <c r="K23" s="27"/>
       <c r="L23" s="26"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="33"/>
+      <c r="O23" s="27"/>
       <c r="P23" s="26"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4">
@@ -1367,7 +1367,7 @@
       <c r="D24" s="5">
         <v>2.1343999999999999</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="36" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="4">
@@ -1376,14 +1376,14 @@
       <c r="H24" s="5">
         <v>3.5375999999999999</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="36" t="s">
         <v>11</v>
       </c>
       <c r="K24" s="4">
         <v>1</v>
       </c>
       <c r="L24" s="5"/>
-      <c r="N24" s="30" t="s">
+      <c r="N24" s="36" t="s">
         <v>14</v>
       </c>
       <c r="O24" s="4">
@@ -1392,130 +1392,130 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="6">
         <v>2</v>
       </c>
       <c r="D25" s="7">
         <v>2.0802999999999998</v>
       </c>
-      <c r="F25" s="31"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="6">
         <v>2</v>
       </c>
       <c r="H25" s="7">
         <v>3.6453000000000002</v>
       </c>
-      <c r="J25" s="31"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="6">
         <v>2</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="N25" s="31"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="6">
         <v>2</v>
       </c>
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="D26" s="7">
         <v>1.9058999999999999</v>
       </c>
-      <c r="F26" s="31"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="H26" s="26">
         <v>3.72</v>
       </c>
-      <c r="J26" s="31"/>
+      <c r="J26" s="37"/>
       <c r="K26" s="6">
         <v>3</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="N26" s="31"/>
+      <c r="N26" s="37"/>
       <c r="O26" s="6">
         <v>3</v>
       </c>
       <c r="P26" s="26"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="6">
         <v>4</v>
       </c>
       <c r="D27" s="7">
         <v>2.0171000000000001</v>
       </c>
-      <c r="F27" s="31"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="6">
         <v>4</v>
       </c>
       <c r="H27" s="26">
         <v>3.7803</v>
       </c>
-      <c r="J27" s="31"/>
+      <c r="J27" s="37"/>
       <c r="K27" s="6">
         <v>4</v>
       </c>
       <c r="L27" s="7"/>
-      <c r="N27" s="31"/>
+      <c r="N27" s="37"/>
       <c r="O27" s="6">
         <v>4</v>
       </c>
       <c r="P27" s="26"/>
     </row>
     <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="32"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="8">
         <v>5</v>
       </c>
       <c r="D28" s="9">
         <v>1.9711000000000001</v>
       </c>
-      <c r="F28" s="32"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="8">
         <v>5</v>
       </c>
       <c r="H28" s="9">
         <v>3.8929999999999998</v>
       </c>
-      <c r="J28" s="32"/>
+      <c r="J28" s="38"/>
       <c r="K28" s="8">
         <v>5</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="N28" s="32"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="8">
         <v>5</v>
       </c>
       <c r="P28" s="9"/>
     </row>
     <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="10">
         <f>AVERAGE(D24:D28)</f>
         <v>2.0217599999999996</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="10">
         <f>AVERAGE(H24:H28)</f>
         <v>3.7152400000000001</v>
       </c>
-      <c r="J29" s="37"/>
-      <c r="K29" s="38"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="29"/>
       <c r="L29" s="10" t="e">
         <f>AVERAGE(L24:L28)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N29" s="37"/>
-      <c r="O29" s="38"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="29"/>
       <c r="P29" s="10" t="e">
         <f>AVERAGE(P24:P28)</f>
         <v>#DIV/0!</v>
@@ -1523,12 +1523,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N8:P9"/>
-    <mergeCell ref="N10:N14"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="N17:N21"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="N24:N28"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B17:B21"/>
@@ -1540,6 +1534,12 @@
     <mergeCell ref="B8:D9"/>
     <mergeCell ref="F8:H9"/>
     <mergeCell ref="J8:L9"/>
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="N10:N14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="N24:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 6000 element dataset test results for Bubble and Merge Sort
</commit_message>
<xml_diff>
--- a/HybridAlgorithmResults.xlsx
+++ b/HybridAlgorithmResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bubble</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>8000 Elements</t>
+  </si>
+  <si>
+    <t>Average Runtime per Number of Elements</t>
   </si>
 </sst>
 </file>
@@ -843,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +859,9 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="39"/>
+      <c r="C2" s="39" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" s="40"/>
       <c r="E2" s="40"/>
       <c r="F2" s="40"/>
@@ -906,7 +911,9 @@
       <c r="D4" s="19">
         <v>24.922080000000001</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="19">
+        <v>55.545540000000003</v>
+      </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -924,7 +931,9 @@
       <c r="D5" s="11">
         <v>3.7152400000000001</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11">
+        <v>5.4830799999999993</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -1232,7 +1241,9 @@
       <c r="K18" s="6">
         <v>2</v>
       </c>
-      <c r="L18" s="7"/>
+      <c r="L18" s="7">
+        <v>54.672600000000003</v>
+      </c>
       <c r="N18" s="37"/>
       <c r="O18" s="6">
         <v>2</v>
@@ -1258,7 +1269,9 @@
       <c r="K19" s="6">
         <v>3</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="7">
+        <v>54.997700000000002</v>
+      </c>
       <c r="N19" s="37"/>
       <c r="O19" s="6">
         <v>3</v>
@@ -1284,7 +1297,9 @@
       <c r="K20" s="6">
         <v>4</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="7">
+        <v>55.184199999999997</v>
+      </c>
       <c r="N20" s="37"/>
       <c r="O20" s="6">
         <v>4</v>
@@ -1310,7 +1325,9 @@
       <c r="K21" s="8">
         <v>5</v>
       </c>
-      <c r="L21" s="9"/>
+      <c r="L21" s="9">
+        <v>57.026800000000001</v>
+      </c>
       <c r="N21" s="38"/>
       <c r="O21" s="8">
         <v>5</v>
@@ -1334,7 +1351,7 @@
       <c r="K22" s="27"/>
       <c r="L22" s="10">
         <f>AVERAGE(L17:L21)</f>
-        <v>55.846400000000003</v>
+        <v>55.545540000000003</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="27"/>
@@ -1382,7 +1399,9 @@
       <c r="K24" s="4">
         <v>1</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="5">
+        <v>5.4630000000000001</v>
+      </c>
       <c r="N24" s="36" t="s">
         <v>14</v>
       </c>
@@ -1410,7 +1429,9 @@
       <c r="K25" s="6">
         <v>2</v>
       </c>
-      <c r="L25" s="7"/>
+      <c r="L25" s="7">
+        <v>5.4660000000000002</v>
+      </c>
       <c r="N25" s="37"/>
       <c r="O25" s="6">
         <v>2</v>
@@ -1436,7 +1457,9 @@
       <c r="K26" s="6">
         <v>3</v>
       </c>
-      <c r="L26" s="7"/>
+      <c r="L26" s="7">
+        <v>5.6996000000000002</v>
+      </c>
       <c r="N26" s="37"/>
       <c r="O26" s="6">
         <v>3</v>
@@ -1462,7 +1485,9 @@
       <c r="K27" s="6">
         <v>4</v>
       </c>
-      <c r="L27" s="7"/>
+      <c r="L27" s="7">
+        <v>5.3846999999999996</v>
+      </c>
       <c r="N27" s="37"/>
       <c r="O27" s="6">
         <v>4</v>
@@ -1488,7 +1513,9 @@
       <c r="K28" s="8">
         <v>5</v>
       </c>
-      <c r="L28" s="9"/>
+      <c r="L28" s="9">
+        <v>5.4020999999999999</v>
+      </c>
       <c r="N28" s="38"/>
       <c r="O28" s="8">
         <v>5</v>
@@ -1510,9 +1537,9 @@
       </c>
       <c r="J29" s="28"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="10" t="e">
+      <c r="L29" s="10">
         <f>AVERAGE(L24:L28)</f>
-        <v>#DIV/0!</v>
+        <v>5.4830799999999993</v>
       </c>
       <c r="N29" s="28"/>
       <c r="O29" s="29"/>

</xml_diff>